<commit_message>
Agrego test scotia - solicitar tarjeta ideal
</commit_message>
<xml_diff>
--- a/src/test/resources/DataTables/DT_AUT_001_DemoTest.xlsx
+++ b/src/test/resources/DataTables/DT_AUT_001_DemoTest.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20398"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50EC2D8-8888-4634-AB72-679940EE63C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB7435F-4721-4D00-8DB9-8A8BC99C3C67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Escenario</t>
   </si>
@@ -110,6 +110,27 @@
   </si>
   <si>
     <t>TC_001_01_EnviarMensaje</t>
+  </si>
+  <si>
+    <t>TC_001_02_SolicitarTarjetaIdeal</t>
+  </si>
+  <si>
+    <t>pPrimerNombre||Lourdes</t>
+  </si>
+  <si>
+    <t>pSegundoNombre||del Mar</t>
+  </si>
+  <si>
+    <t>pPrimerApellido||Lede</t>
+  </si>
+  <si>
+    <t>pHomoclave||123</t>
+  </si>
+  <si>
+    <t>pFechaNacimiento||17021998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pSegundoApellido|| </t>
   </si>
 </sst>
 </file>
@@ -154,9 +175,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -458,9 +478,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" customWidth="1"/>
     <col min="5" max="5" width="37" customWidth="1"/>
     <col min="6" max="6" width="22.5703125" customWidth="1"/>
@@ -524,232 +544,249 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
     </row>
     <row r="17" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
     </row>
     <row r="18" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
     </row>
     <row r="19" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
     </row>
     <row r="20" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
     </row>
     <row r="21" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
     </row>
     <row r="22" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Selenium y Gherking - Solicitud tarjeta ideal test
</commit_message>
<xml_diff>
--- a/src/test/resources/DataTables/DT_AUT_001_DemoTest.xlsx
+++ b/src/test/resources/DataTables/DT_AUT_001_DemoTest.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20398"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB7435F-4721-4D00-8DB9-8A8BC99C3C67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F015332-6192-4804-8EDD-DEFF23A4D7BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -473,7 +473,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>